<commit_message>
Added error types and codes. Corrected a bug in CachedStructure. Finalised ExcelParser. Started ExcelTemplateParser. Moved newTransaction() to SessionObject to allow nested transactions. Finalised up to and including template structure validation.
</commit_message>
<xml_diff>
--- a/Library/test/CWR_Checklist_Template.test.xlsx
+++ b/Library/test/CWR_Checklist_Template.test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="1"/>
+    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Read this" sheetId="13" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="423">
   <si>
     <t xml:space="preserve">Country code identifying the National CWR checklist; the code of the country preparing the CWR checklist. For country codes use the three-letter ISO 3166-1 (see: http://unstats.un.org/unsd/methods/m49/m49alpha.htm ) </t>
   </si>
@@ -2151,6 +2151,93 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>Test dataset</t>
+  </si>
+  <si>
+    <t>http://pgrdiversity.bioversityinternational.org</t>
+  </si>
+  <si>
+    <t>This is a trial dataset used to test template import.</t>
+  </si>
+  <si>
+    <t>ITA406</t>
+  </si>
+  <si>
+    <t>IT-RM</t>
+  </si>
+  <si>
+    <t>TEST-1</t>
+  </si>
+  <si>
+    <t>http://bioversityinternational.org</t>
+  </si>
+  <si>
+    <t>Plantae</t>
+  </si>
+  <si>
+    <t>Triticum</t>
+  </si>
+  <si>
+    <t>aestivum</t>
+  </si>
+  <si>
+    <t>L.</t>
+  </si>
+  <si>
+    <t>var. ajutense</t>
+  </si>
+  <si>
+    <t>Triticum aestivum L. var. ajutense</t>
+  </si>
+  <si>
+    <t>http://www.ars-grin.gov/cgi-bin/npgs/html/taxon.pl?470028</t>
+  </si>
+  <si>
+    <t>GRIN Taxonomy for Plants</t>
+  </si>
+  <si>
+    <t>Triticum aestivum L. subsp. aestivum</t>
+  </si>
+  <si>
+    <t>en@wheat;it@grano</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Test 1 record</t>
+  </si>
+  <si>
+    <t>Triticum vulgare;Triticum muticum</t>
+  </si>
+  <si>
+    <t>forced;spontaneous</t>
+  </si>
+  <si>
+    <t>85;75</t>
+  </si>
+  <si>
+    <t>Maccarese</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>MACCA-3</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>G5</t>
   </si>
 </sst>
 </file>
@@ -2545,7 +2632,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="106">
+  <cellStyleXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2652,8 +2739,10 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2841,10 +2930,16 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="106" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="106">
+  <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2897,6 +2992,7 @@
     <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -2950,6 +3046,7 @@
     <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4355,7 +4452,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="23">
-      <c r="A1" s="72"/>
+      <c r="A1" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4372,11 +4469,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AS8"/>
+  <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5097,7 +5194,97 @@
         <v>258</v>
       </c>
     </row>
+    <row r="9" spans="1:45" ht="28">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="C9" s="72" t="s">
+        <v>395</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="I9" s="72" t="s">
+        <v>400</v>
+      </c>
+      <c r="J9" s="73">
+        <v>42069</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="L9" s="25">
+        <v>201503</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="N9" s="25">
+        <v>2</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="T9" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="U9" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="V9" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="W9" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="Y9" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="Z9" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="AA9" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="AB9" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="AC9" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="AD9" s="25" t="s">
+        <v>410</v>
+      </c>
+      <c r="AE9" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>412</v>
+      </c>
+      <c r="AP9">
+        <v>30</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>413</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1"/>
+    <hyperlink ref="I9" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0"/>
   <extLst>
@@ -5111,11 +5298,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5229,6 +5416,20 @@
       </c>
       <c r="F8" s="63" t="s">
         <v>325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -5245,11 +5446,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5576,6 +5777,41 @@
       </c>
       <c r="T8" s="59" t="s">
         <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="25">
+        <v>2</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>417</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>418</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>419</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>420</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="I9" s="25">
+        <v>2</v>
+      </c>
+      <c r="J9" s="25">
+        <v>2015</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="S9" s="25">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -5627,7 +5863,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="56">
-      <c r="A2" s="71"/>
+      <c r="A2" s="74"/>
       <c r="B2" s="20" t="s">
         <v>145</v>
       </c>
@@ -5640,7 +5876,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="42">
-      <c r="A3" s="71"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5655,7 +5891,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="140">
-      <c r="A4" s="71"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="5" t="s">
         <v>99</v>
       </c>
@@ -5670,7 +5906,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="70">
-      <c r="A5" s="71"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="5" t="s">
         <v>100</v>
       </c>
@@ -5685,7 +5921,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="98">
-      <c r="A6" s="71"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="5" t="s">
         <v>101</v>
       </c>
@@ -5698,7 +5934,7 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="42">
-      <c r="A7" s="71"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="5" t="s">
         <v>102</v>
       </c>
@@ -5711,7 +5947,7 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="28">
-      <c r="A8" s="71"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="5" t="s">
         <v>142</v>
       </c>
@@ -5724,7 +5960,7 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="56">
-      <c r="A9" s="71"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="16" t="s">
         <v>103</v>
       </c>
@@ -5737,7 +5973,7 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="71"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="5" t="s">
         <v>98</v>
       </c>
@@ -5750,7 +5986,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="28">
-      <c r="A11" s="71"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="5" t="s">
         <v>104</v>
       </c>
@@ -5763,7 +5999,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="28">
-      <c r="A12" s="71"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="5" t="s">
         <v>105</v>
       </c>
@@ -5776,7 +6012,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28">
-      <c r="A13" s="71"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="5" t="s">
         <v>106</v>
       </c>
@@ -5789,7 +6025,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28">
-      <c r="A14" s="71"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="5" t="s">
         <v>107</v>
       </c>
@@ -5802,7 +6038,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="71"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="5" t="s">
         <v>108</v>
       </c>
@@ -5817,7 +6053,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="28">
-      <c r="A16" s="71"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="5" t="s">
         <v>109</v>
       </c>
@@ -5832,7 +6068,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="71"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="5" t="s">
         <v>110</v>
       </c>
@@ -5847,7 +6083,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="56">
-      <c r="A18" s="71"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="5" t="s">
         <v>111</v>
       </c>
@@ -5862,7 +6098,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="71"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="5" t="s">
         <v>112</v>
       </c>
@@ -5877,7 +6113,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="28">
-      <c r="A20" s="71"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="5" t="s">
         <v>113</v>
       </c>
@@ -5892,7 +6128,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="70">
-      <c r="A21" s="71"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="5" t="s">
         <v>114</v>
       </c>
@@ -5905,7 +6141,7 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="42">
-      <c r="A22" s="71"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="5" t="s">
         <v>115</v>
       </c>
@@ -5920,7 +6156,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="28">
-      <c r="A23" s="71"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="5" t="s">
         <v>116</v>
       </c>
@@ -5933,7 +6169,7 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="120" customHeight="1">
-      <c r="A24" s="71"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="22" t="s">
         <v>151</v>
       </c>
@@ -5950,7 +6186,7 @@
       <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" ht="36">
-      <c r="A25" s="71"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="5" t="s">
         <v>117</v>
       </c>
@@ -5967,7 +6203,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="60">
-      <c r="A26" s="71"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="5" t="s">
         <v>118</v>
       </c>
@@ -5982,7 +6218,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="28">
-      <c r="A27" s="71"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="5" t="s">
         <v>119</v>
       </c>
@@ -5995,7 +6231,7 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="56">
-      <c r="A28" s="71"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="5" t="s">
         <v>120</v>
       </c>
@@ -6008,7 +6244,7 @@
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="28">
-      <c r="A29" s="71"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="5" t="s">
         <v>122</v>
       </c>
@@ -6021,7 +6257,7 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="112">
-      <c r="A30" s="71"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="5" t="s">
         <v>121</v>
       </c>
@@ -6034,7 +6270,7 @@
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:7" ht="28">
-      <c r="A31" s="71"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="5" t="s">
         <v>123</v>
       </c>
@@ -6060,7 +6296,7 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="56">
-      <c r="A33" s="71"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="20" t="s">
         <v>145</v>
       </c>
@@ -6073,7 +6309,7 @@
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" ht="28">
-      <c r="A34" s="71"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="5" t="s">
         <v>125</v>
       </c>
@@ -6086,7 +6322,7 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="28">
-      <c r="A35" s="71"/>
+      <c r="A35" s="74"/>
       <c r="B35" s="5" t="s">
         <v>127</v>
       </c>
@@ -6099,7 +6335,7 @@
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="56">
-      <c r="A36" s="71"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="5" t="s">
         <v>126</v>
       </c>
@@ -6112,7 +6348,7 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="28">
-      <c r="A37" s="71"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="5" t="s">
         <v>128</v>
       </c>
@@ -6138,7 +6374,7 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="56">
-      <c r="A39" s="71"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="20" t="s">
         <v>145</v>
       </c>
@@ -6151,7 +6387,7 @@
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="71"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="5" t="s">
         <v>130</v>
       </c>
@@ -6166,7 +6402,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="42">
-      <c r="A41" s="71"/>
+      <c r="A41" s="74"/>
       <c r="B41" s="5" t="s">
         <v>131</v>
       </c>
@@ -6179,7 +6415,7 @@
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" ht="84">
-      <c r="A42" s="71"/>
+      <c r="A42" s="74"/>
       <c r="B42" s="5" t="s">
         <v>132</v>
       </c>
@@ -6192,7 +6428,7 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" ht="56">
-      <c r="A43" s="71"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="5" t="s">
         <v>133</v>
       </c>
@@ -6205,7 +6441,7 @@
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="56">
-      <c r="A44" s="71"/>
+      <c r="A44" s="74"/>
       <c r="B44" s="5" t="s">
         <v>134</v>
       </c>
@@ -6218,7 +6454,7 @@
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="56">
-      <c r="A45" s="71"/>
+      <c r="A45" s="74"/>
       <c r="B45" s="5" t="s">
         <v>134</v>
       </c>
@@ -6231,7 +6467,7 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="29">
-      <c r="A46" s="71"/>
+      <c r="A46" s="74"/>
       <c r="B46" s="5" t="s">
         <v>135</v>
       </c>
@@ -6244,7 +6480,7 @@
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="42">
-      <c r="A47" s="71"/>
+      <c r="A47" s="74"/>
       <c r="B47" s="5" t="s">
         <v>136</v>
       </c>
@@ -6257,7 +6493,7 @@
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" ht="406">
-      <c r="A48" s="71"/>
+      <c r="A48" s="74"/>
       <c r="B48" s="5" t="s">
         <v>137</v>
       </c>
@@ -6270,7 +6506,7 @@
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" ht="266">
-      <c r="A49" s="71"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="5" t="s">
         <v>138</v>
       </c>
@@ -6283,7 +6519,7 @@
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" ht="70">
-      <c r="A50" s="71"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="5" t="s">
         <v>139</v>
       </c>
@@ -6296,7 +6532,7 @@
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" ht="42">
-      <c r="A51" s="71" t="s">
+      <c r="A51" s="74" t="s">
         <v>155</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -6311,7 +6547,7 @@
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="70">
-      <c r="A52" s="71"/>
+      <c r="A52" s="74"/>
       <c r="B52" s="5" t="s">
         <v>141</v>
       </c>
@@ -6324,7 +6560,7 @@
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="56">
-      <c r="A53" s="71"/>
+      <c r="A53" s="74"/>
       <c r="B53" s="5"/>
       <c r="C53" s="3" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
Finalised upload and session progress services, need to add fail case. Transactions now do not need session, only transactions created by sessions have this reference: this is to allow selection of root level transactions for progress.
</commit_message>
<xml_diff>
--- a/Library/test/CWR_Checklist_Template.test.xlsx
+++ b/Library/test/CWR_Checklist_Template.test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="2"/>
+    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Read this" sheetId="13" r:id="rId1"/>
@@ -2931,13 +2931,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="106" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4471,7 +4471,7 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
@@ -5201,7 +5201,7 @@
       <c r="B9" s="25" t="s">
         <v>394</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="73" t="s">
         <v>395</v>
       </c>
       <c r="D9" s="25" t="s">
@@ -5216,10 +5216,10 @@
       <c r="G9" s="25" t="s">
         <v>397</v>
       </c>
-      <c r="I9" s="72" t="s">
+      <c r="I9" s="73" t="s">
         <v>400</v>
       </c>
-      <c r="J9" s="73">
+      <c r="J9" s="74">
         <v>42069</v>
       </c>
       <c r="K9" s="25" t="s">
@@ -5300,7 +5300,7 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
@@ -5863,7 +5863,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="56">
-      <c r="A2" s="74"/>
+      <c r="A2" s="72"/>
       <c r="B2" s="20" t="s">
         <v>145</v>
       </c>
@@ -5876,7 +5876,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="42">
-      <c r="A3" s="74"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5891,7 +5891,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="140">
-      <c r="A4" s="74"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="5" t="s">
         <v>99</v>
       </c>
@@ -5906,7 +5906,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="70">
-      <c r="A5" s="74"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="5" t="s">
         <v>100</v>
       </c>
@@ -5921,7 +5921,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="98">
-      <c r="A6" s="74"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="5" t="s">
         <v>101</v>
       </c>
@@ -5934,7 +5934,7 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="42">
-      <c r="A7" s="74"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="5" t="s">
         <v>102</v>
       </c>
@@ -5947,7 +5947,7 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="28">
-      <c r="A8" s="74"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="5" t="s">
         <v>142</v>
       </c>
@@ -5960,7 +5960,7 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="56">
-      <c r="A9" s="74"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="16" t="s">
         <v>103</v>
       </c>
@@ -5973,7 +5973,7 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="74"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="5" t="s">
         <v>98</v>
       </c>
@@ -5986,7 +5986,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="28">
-      <c r="A11" s="74"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="5" t="s">
         <v>104</v>
       </c>
@@ -5999,7 +5999,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="28">
-      <c r="A12" s="74"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="5" t="s">
         <v>105</v>
       </c>
@@ -6012,7 +6012,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28">
-      <c r="A13" s="74"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="5" t="s">
         <v>106</v>
       </c>
@@ -6025,7 +6025,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28">
-      <c r="A14" s="74"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="5" t="s">
         <v>107</v>
       </c>
@@ -6038,7 +6038,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="74"/>
+      <c r="A15" s="72"/>
       <c r="B15" s="5" t="s">
         <v>108</v>
       </c>
@@ -6053,7 +6053,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="28">
-      <c r="A16" s="74"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="5" t="s">
         <v>109</v>
       </c>
@@ -6068,7 +6068,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="74"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="5" t="s">
         <v>110</v>
       </c>
@@ -6083,7 +6083,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="56">
-      <c r="A18" s="74"/>
+      <c r="A18" s="72"/>
       <c r="B18" s="5" t="s">
         <v>111</v>
       </c>
@@ -6098,7 +6098,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="74"/>
+      <c r="A19" s="72"/>
       <c r="B19" s="5" t="s">
         <v>112</v>
       </c>
@@ -6113,7 +6113,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="28">
-      <c r="A20" s="74"/>
+      <c r="A20" s="72"/>
       <c r="B20" s="5" t="s">
         <v>113</v>
       </c>
@@ -6128,7 +6128,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="70">
-      <c r="A21" s="74"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="5" t="s">
         <v>114</v>
       </c>
@@ -6141,7 +6141,7 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="42">
-      <c r="A22" s="74"/>
+      <c r="A22" s="72"/>
       <c r="B22" s="5" t="s">
         <v>115</v>
       </c>
@@ -6156,7 +6156,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="28">
-      <c r="A23" s="74"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="5" t="s">
         <v>116</v>
       </c>
@@ -6169,7 +6169,7 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="120" customHeight="1">
-      <c r="A24" s="74"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="22" t="s">
         <v>151</v>
       </c>
@@ -6186,7 +6186,7 @@
       <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" ht="36">
-      <c r="A25" s="74"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="5" t="s">
         <v>117</v>
       </c>
@@ -6203,7 +6203,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="60">
-      <c r="A26" s="74"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="5" t="s">
         <v>118</v>
       </c>
@@ -6218,7 +6218,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="28">
-      <c r="A27" s="74"/>
+      <c r="A27" s="72"/>
       <c r="B27" s="5" t="s">
         <v>119</v>
       </c>
@@ -6231,7 +6231,7 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="56">
-      <c r="A28" s="74"/>
+      <c r="A28" s="72"/>
       <c r="B28" s="5" t="s">
         <v>120</v>
       </c>
@@ -6244,7 +6244,7 @@
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="28">
-      <c r="A29" s="74"/>
+      <c r="A29" s="72"/>
       <c r="B29" s="5" t="s">
         <v>122</v>
       </c>
@@ -6257,7 +6257,7 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="112">
-      <c r="A30" s="74"/>
+      <c r="A30" s="72"/>
       <c r="B30" s="5" t="s">
         <v>121</v>
       </c>
@@ -6270,7 +6270,7 @@
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:7" ht="28">
-      <c r="A31" s="74"/>
+      <c r="A31" s="72"/>
       <c r="B31" s="5" t="s">
         <v>123</v>
       </c>
@@ -6296,7 +6296,7 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="56">
-      <c r="A33" s="74"/>
+      <c r="A33" s="72"/>
       <c r="B33" s="20" t="s">
         <v>145</v>
       </c>
@@ -6309,7 +6309,7 @@
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" ht="28">
-      <c r="A34" s="74"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="5" t="s">
         <v>125</v>
       </c>
@@ -6322,7 +6322,7 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="28">
-      <c r="A35" s="74"/>
+      <c r="A35" s="72"/>
       <c r="B35" s="5" t="s">
         <v>127</v>
       </c>
@@ -6335,7 +6335,7 @@
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="56">
-      <c r="A36" s="74"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="5" t="s">
         <v>126</v>
       </c>
@@ -6348,7 +6348,7 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="28">
-      <c r="A37" s="74"/>
+      <c r="A37" s="72"/>
       <c r="B37" s="5" t="s">
         <v>128</v>
       </c>
@@ -6374,7 +6374,7 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="56">
-      <c r="A39" s="74"/>
+      <c r="A39" s="72"/>
       <c r="B39" s="20" t="s">
         <v>145</v>
       </c>
@@ -6387,7 +6387,7 @@
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="74"/>
+      <c r="A40" s="72"/>
       <c r="B40" s="5" t="s">
         <v>130</v>
       </c>
@@ -6402,7 +6402,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="42">
-      <c r="A41" s="74"/>
+      <c r="A41" s="72"/>
       <c r="B41" s="5" t="s">
         <v>131</v>
       </c>
@@ -6415,7 +6415,7 @@
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" ht="84">
-      <c r="A42" s="74"/>
+      <c r="A42" s="72"/>
       <c r="B42" s="5" t="s">
         <v>132</v>
       </c>
@@ -6428,7 +6428,7 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" ht="56">
-      <c r="A43" s="74"/>
+      <c r="A43" s="72"/>
       <c r="B43" s="5" t="s">
         <v>133</v>
       </c>
@@ -6441,7 +6441,7 @@
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="56">
-      <c r="A44" s="74"/>
+      <c r="A44" s="72"/>
       <c r="B44" s="5" t="s">
         <v>134</v>
       </c>
@@ -6454,7 +6454,7 @@
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="56">
-      <c r="A45" s="74"/>
+      <c r="A45" s="72"/>
       <c r="B45" s="5" t="s">
         <v>134</v>
       </c>
@@ -6467,7 +6467,7 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="29">
-      <c r="A46" s="74"/>
+      <c r="A46" s="72"/>
       <c r="B46" s="5" t="s">
         <v>135</v>
       </c>
@@ -6480,7 +6480,7 @@
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="42">
-      <c r="A47" s="74"/>
+      <c r="A47" s="72"/>
       <c r="B47" s="5" t="s">
         <v>136</v>
       </c>
@@ -6493,7 +6493,7 @@
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" ht="406">
-      <c r="A48" s="74"/>
+      <c r="A48" s="72"/>
       <c r="B48" s="5" t="s">
         <v>137</v>
       </c>
@@ -6506,7 +6506,7 @@
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" ht="266">
-      <c r="A49" s="74"/>
+      <c r="A49" s="72"/>
       <c r="B49" s="5" t="s">
         <v>138</v>
       </c>
@@ -6519,7 +6519,7 @@
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" ht="70">
-      <c r="A50" s="74"/>
+      <c r="A50" s="72"/>
       <c r="B50" s="5" t="s">
         <v>139</v>
       </c>
@@ -6532,7 +6532,7 @@
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" ht="42">
-      <c r="A51" s="74" t="s">
+      <c r="A51" s="72" t="s">
         <v>155</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -6547,7 +6547,7 @@
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="70">
-      <c r="A52" s="74"/>
+      <c r="A52" s="72"/>
       <c r="B52" s="5" t="s">
         <v>141</v>
       </c>
@@ -6560,7 +6560,7 @@
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="56">
-      <c r="A53" s="74"/>
+      <c r="A53" s="72"/>
       <c r="B53" s="5"/>
       <c r="C53" s="3" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
Need to refactor session progress service.
</commit_message>
<xml_diff>
--- a/Library/test/CWR_Checklist_Template.test.xlsx
+++ b/Library/test/CWR_Checklist_Template.test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="1"/>
+    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Read this" sheetId="13" r:id="rId1"/>
@@ -2931,13 +2931,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="106" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4471,7 +4471,7 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
@@ -5201,7 +5201,7 @@
       <c r="B9" s="25" t="s">
         <v>394</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="72" t="s">
         <v>395</v>
       </c>
       <c r="D9" s="25" t="s">
@@ -5216,10 +5216,10 @@
       <c r="G9" s="25" t="s">
         <v>397</v>
       </c>
-      <c r="I9" s="73" t="s">
+      <c r="I9" s="72" t="s">
         <v>400</v>
       </c>
-      <c r="J9" s="74">
+      <c r="J9" s="73">
         <v>42069</v>
       </c>
       <c r="K9" s="25" t="s">
@@ -5300,7 +5300,7 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
@@ -5863,7 +5863,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="56">
-      <c r="A2" s="72"/>
+      <c r="A2" s="74"/>
       <c r="B2" s="20" t="s">
         <v>145</v>
       </c>
@@ -5876,7 +5876,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="42">
-      <c r="A3" s="72"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5891,7 +5891,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="140">
-      <c r="A4" s="72"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="5" t="s">
         <v>99</v>
       </c>
@@ -5906,7 +5906,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="70">
-      <c r="A5" s="72"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="5" t="s">
         <v>100</v>
       </c>
@@ -5921,7 +5921,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="98">
-      <c r="A6" s="72"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="5" t="s">
         <v>101</v>
       </c>
@@ -5934,7 +5934,7 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="42">
-      <c r="A7" s="72"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="5" t="s">
         <v>102</v>
       </c>
@@ -5947,7 +5947,7 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="28">
-      <c r="A8" s="72"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="5" t="s">
         <v>142</v>
       </c>
@@ -5960,7 +5960,7 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="56">
-      <c r="A9" s="72"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="16" t="s">
         <v>103</v>
       </c>
@@ -5973,7 +5973,7 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="72"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="5" t="s">
         <v>98</v>
       </c>
@@ -5986,7 +5986,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="28">
-      <c r="A11" s="72"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="5" t="s">
         <v>104</v>
       </c>
@@ -5999,7 +5999,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="28">
-      <c r="A12" s="72"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="5" t="s">
         <v>105</v>
       </c>
@@ -6012,7 +6012,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28">
-      <c r="A13" s="72"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="5" t="s">
         <v>106</v>
       </c>
@@ -6025,7 +6025,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28">
-      <c r="A14" s="72"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="5" t="s">
         <v>107</v>
       </c>
@@ -6038,7 +6038,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="72"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="5" t="s">
         <v>108</v>
       </c>
@@ -6053,7 +6053,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="28">
-      <c r="A16" s="72"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="5" t="s">
         <v>109</v>
       </c>
@@ -6068,7 +6068,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="72"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="5" t="s">
         <v>110</v>
       </c>
@@ -6083,7 +6083,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="56">
-      <c r="A18" s="72"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="5" t="s">
         <v>111</v>
       </c>
@@ -6098,7 +6098,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="72"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="5" t="s">
         <v>112</v>
       </c>
@@ -6113,7 +6113,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="28">
-      <c r="A20" s="72"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="5" t="s">
         <v>113</v>
       </c>
@@ -6128,7 +6128,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="70">
-      <c r="A21" s="72"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="5" t="s">
         <v>114</v>
       </c>
@@ -6141,7 +6141,7 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="42">
-      <c r="A22" s="72"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="5" t="s">
         <v>115</v>
       </c>
@@ -6156,7 +6156,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="28">
-      <c r="A23" s="72"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="5" t="s">
         <v>116</v>
       </c>
@@ -6169,7 +6169,7 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="120" customHeight="1">
-      <c r="A24" s="72"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="22" t="s">
         <v>151</v>
       </c>
@@ -6186,7 +6186,7 @@
       <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" ht="36">
-      <c r="A25" s="72"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="5" t="s">
         <v>117</v>
       </c>
@@ -6203,7 +6203,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="60">
-      <c r="A26" s="72"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="5" t="s">
         <v>118</v>
       </c>
@@ -6218,7 +6218,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="28">
-      <c r="A27" s="72"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="5" t="s">
         <v>119</v>
       </c>
@@ -6231,7 +6231,7 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="56">
-      <c r="A28" s="72"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="5" t="s">
         <v>120</v>
       </c>
@@ -6244,7 +6244,7 @@
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="28">
-      <c r="A29" s="72"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="5" t="s">
         <v>122</v>
       </c>
@@ -6257,7 +6257,7 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="112">
-      <c r="A30" s="72"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="5" t="s">
         <v>121</v>
       </c>
@@ -6270,7 +6270,7 @@
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:7" ht="28">
-      <c r="A31" s="72"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="5" t="s">
         <v>123</v>
       </c>
@@ -6296,7 +6296,7 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="56">
-      <c r="A33" s="72"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="20" t="s">
         <v>145</v>
       </c>
@@ -6309,7 +6309,7 @@
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" ht="28">
-      <c r="A34" s="72"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="5" t="s">
         <v>125</v>
       </c>
@@ -6322,7 +6322,7 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="28">
-      <c r="A35" s="72"/>
+      <c r="A35" s="74"/>
       <c r="B35" s="5" t="s">
         <v>127</v>
       </c>
@@ -6335,7 +6335,7 @@
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="56">
-      <c r="A36" s="72"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="5" t="s">
         <v>126</v>
       </c>
@@ -6348,7 +6348,7 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="28">
-      <c r="A37" s="72"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="5" t="s">
         <v>128</v>
       </c>
@@ -6374,7 +6374,7 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="56">
-      <c r="A39" s="72"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="20" t="s">
         <v>145</v>
       </c>
@@ -6387,7 +6387,7 @@
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="72"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="5" t="s">
         <v>130</v>
       </c>
@@ -6402,7 +6402,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="42">
-      <c r="A41" s="72"/>
+      <c r="A41" s="74"/>
       <c r="B41" s="5" t="s">
         <v>131</v>
       </c>
@@ -6415,7 +6415,7 @@
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" ht="84">
-      <c r="A42" s="72"/>
+      <c r="A42" s="74"/>
       <c r="B42" s="5" t="s">
         <v>132</v>
       </c>
@@ -6428,7 +6428,7 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" ht="56">
-      <c r="A43" s="72"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="5" t="s">
         <v>133</v>
       </c>
@@ -6441,7 +6441,7 @@
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="56">
-      <c r="A44" s="72"/>
+      <c r="A44" s="74"/>
       <c r="B44" s="5" t="s">
         <v>134</v>
       </c>
@@ -6454,7 +6454,7 @@
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="56">
-      <c r="A45" s="72"/>
+      <c r="A45" s="74"/>
       <c r="B45" s="5" t="s">
         <v>134</v>
       </c>
@@ -6467,7 +6467,7 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="29">
-      <c r="A46" s="72"/>
+      <c r="A46" s="74"/>
       <c r="B46" s="5" t="s">
         <v>135</v>
       </c>
@@ -6480,7 +6480,7 @@
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="42">
-      <c r="A47" s="72"/>
+      <c r="A47" s="74"/>
       <c r="B47" s="5" t="s">
         <v>136</v>
       </c>
@@ -6493,7 +6493,7 @@
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" ht="406">
-      <c r="A48" s="72"/>
+      <c r="A48" s="74"/>
       <c r="B48" s="5" t="s">
         <v>137</v>
       </c>
@@ -6506,7 +6506,7 @@
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" ht="266">
-      <c r="A49" s="72"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="5" t="s">
         <v>138</v>
       </c>
@@ -6519,7 +6519,7 @@
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" ht="70">
-      <c r="A50" s="72"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="5" t="s">
         <v>139</v>
       </c>
@@ -6532,7 +6532,7 @@
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" ht="42">
-      <c r="A51" s="72" t="s">
+      <c r="A51" s="74" t="s">
         <v>155</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -6547,7 +6547,7 @@
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="70">
-      <c r="A52" s="72"/>
+      <c r="A52" s="74"/>
       <c r="B52" s="5" t="s">
         <v>141</v>
       </c>
@@ -6560,7 +6560,7 @@
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="56">
-      <c r="A53" s="72"/>
+      <c r="A53" s="74"/>
       <c r="B53" s="5"/>
       <c r="C53" s="3" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
Finalised worksheet data validation and storage. Removed collection name from transformation records: the tag determines which collection should be probed. Moved data validation routines from SessionUpload class to functions.
</commit_message>
<xml_diff>
--- a/Library/test/CWR_Checklist_Template.test.xlsx
+++ b/Library/test/CWR_Checklist_Template.test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="724" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Read this" sheetId="13" r:id="rId1"/>
@@ -1261,9 +1261,6 @@
     <t>CK_CWRCODE</t>
   </si>
   <si>
-    <t>Country or region code identifying the National CWR checklist, or the code of the country preparing the CWR checklist. For country codes use the three-letter ISO 3166-1 (see: http://unstats.un.org/unsd/methods/m49/m49alpha.htm); for region codes use the ISO 3166-2 standard (see http://en.wikipedia.org/wiki/Category:ISO_3166 in section 2).</t>
-  </si>
-  <si>
     <t>ESP for Spain
 GBR for United Kingdom
 ES-AN for the autonomous community of Andalucía
@@ -2358,6 +2355,9 @@
   </si>
   <si>
     <t>reference</t>
+  </si>
+  <si>
+    <t>Country or region code identifying the  CWR checklist, or the code of the country preparing the CWR checklist. For country codes use the three-letter ISO 3166-1 (see: http://unstats.un.org/unsd/methods/m49/m49alpha.htm); for region codes use the ISO 3166-2 standard (see http://en.wikipedia.org/wiki/Category:ISO_3166 in section 2).</t>
   </si>
 </sst>
 </file>
@@ -2576,7 +2576,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2591,6 +2591,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2862,7 +2868,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3058,6 +3064,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4591,9 +4612,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4757,133 +4778,133 @@
         <v>173</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>295</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>297</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>299</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>302</v>
+        <v>294</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>296</v>
+      </c>
+      <c r="F4" s="75" t="s">
+        <v>298</v>
+      </c>
+      <c r="G4" s="75" t="s">
+        <v>301</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K4" s="65" t="s">
         <v>175</v>
       </c>
       <c r="L4" s="65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M4" s="66" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N4" s="66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O4" s="64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P4" s="64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q4" s="64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R4" s="64" t="s">
+        <v>203</v>
+      </c>
+      <c r="S4" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="S4" s="64" t="s">
-        <v>205</v>
-      </c>
       <c r="T4" s="64" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U4" s="64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="V4" s="64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="W4" s="64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X4" s="64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y4" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Z4" s="64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA4" s="64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AB4" s="64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AC4" s="64" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AD4" s="64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AE4" s="64" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AF4" s="64" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AG4" s="64" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AH4" s="64" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AI4" s="64" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AJ4" s="64" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AK4" s="64" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AL4" s="64" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AM4" s="64" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AN4" s="64" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AO4" s="64" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AP4" s="64" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AQ4" s="64" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AR4" s="65" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AS4" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:45" s="28" customFormat="1" ht="154">
@@ -4894,40 +4915,40 @@
         <v>174</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>294</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>298</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>301</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>304</v>
+        <v>293</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>297</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>300</v>
+      </c>
+      <c r="G5" s="76" t="s">
+        <v>303</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I5" s="41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J5" s="41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K5" s="41" t="s">
-        <v>177</v>
+        <v>462</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M5" s="42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N5" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
@@ -4935,43 +4956,43 @@
       <c r="R5" s="34"/>
       <c r="S5" s="34"/>
       <c r="T5" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U5" s="34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V5" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="W5" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="X5" s="43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Y5" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z5" s="34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA5" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AB5" s="34" t="s">
         <v>32</v>
       </c>
       <c r="AC5" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AD5" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AE5" s="34" t="s">
         <v>37</v>
       </c>
       <c r="AF5" s="34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AG5" s="34" t="s">
         <v>39</v>
@@ -4983,34 +5004,34 @@
         <v>40</v>
       </c>
       <c r="AJ5" s="34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AK5" s="34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AL5" s="34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AM5" s="34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AN5" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AO5" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AP5" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AQ5" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AR5" s="34" t="s">
         <v>50</v>
       </c>
       <c r="AS5" s="51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:45" s="29" customFormat="1" ht="70">
@@ -5018,24 +5039,24 @@
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>186</v>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" s="77" t="s">
+        <v>185</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
       <c r="K6" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N6" s="35">
         <v>2</v>
@@ -5056,35 +5077,35 @@
         <v>19</v>
       </c>
       <c r="T6" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U6" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V6" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="W6" s="43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X6" s="43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Y6" s="36"/>
       <c r="Z6" s="36" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AA6" s="43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AB6" s="43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AC6" s="43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AD6" s="43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AE6" s="43"/>
       <c r="AF6" s="43"/>
@@ -5092,17 +5113,17 @@
       <c r="AH6" s="43"/>
       <c r="AI6" s="43"/>
       <c r="AJ6" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AK6" s="43"/>
       <c r="AL6" s="43" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AM6" s="43"/>
       <c r="AN6" s="43"/>
       <c r="AO6" s="43"/>
       <c r="AP6" s="43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AQ6" s="43"/>
       <c r="AR6" s="43"/>
@@ -5110,32 +5131,32 @@
     </row>
     <row r="7" spans="1:45" s="29" customFormat="1">
       <c r="A7" s="54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
       <c r="J7" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K7" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L7" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M7" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N7" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O7" s="37"/>
       <c r="P7" s="37"/>
@@ -5143,18 +5164,18 @@
       <c r="R7" s="37"/>
       <c r="S7" s="37"/>
       <c r="T7" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U7" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V7" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="W7" s="37"/>
       <c r="X7" s="38"/>
       <c r="Y7" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z7" s="37"/>
       <c r="AA7" s="37"/>
@@ -5182,136 +5203,136 @@
         <v>172</v>
       </c>
       <c r="B8" s="57" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="57" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="57" t="s">
-        <v>290</v>
-      </c>
       <c r="D8" s="57" t="s">
-        <v>293</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>296</v>
-      </c>
-      <c r="F8" s="57" t="s">
-        <v>300</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>303</v>
+        <v>292</v>
+      </c>
+      <c r="E8" s="79" t="s">
+        <v>295</v>
+      </c>
+      <c r="F8" s="79" t="s">
+        <v>299</v>
+      </c>
+      <c r="G8" s="79" t="s">
+        <v>302</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K8" s="57" t="s">
         <v>176</v>
       </c>
       <c r="L8" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="M8" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="M8" s="57" t="s">
-        <v>184</v>
-      </c>
       <c r="N8" s="57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P8" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q8" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="Q8" s="57" t="s">
-        <v>201</v>
-      </c>
       <c r="R8" s="58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S8" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="T8" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="T8" s="58" t="s">
-        <v>207</v>
-      </c>
       <c r="U8" s="58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V8" s="58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="W8" s="58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X8" s="58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y8" s="57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Z8" s="57" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AA8" s="58" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AB8" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AC8" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AD8" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AE8" s="58" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AF8" s="58" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AG8" s="58" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AH8" s="58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AI8" s="58" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AJ8" s="58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AK8" s="58" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL8" s="58" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AM8" s="58" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AN8" s="58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AO8" s="58" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AP8" s="58" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AQ8" s="58" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AR8" s="58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AS8" s="59" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:45" ht="28">
@@ -5319,133 +5340,133 @@
         <v>1</v>
       </c>
       <c r="B9" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C9" s="72" t="s">
         <v>394</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="D9" s="25" t="s">
         <v>395</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="E9" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>396</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>399</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="G9" s="25" t="s">
+      <c r="I9" s="72" t="s">
+        <v>444</v>
+      </c>
+      <c r="J9" s="73" t="s">
+        <v>426</v>
+      </c>
+      <c r="K9" s="25" t="s">
         <v>397</v>
-      </c>
-      <c r="I9" s="72" t="s">
-        <v>445</v>
-      </c>
-      <c r="J9" s="73" t="s">
-        <v>427</v>
-      </c>
-      <c r="K9" s="25" t="s">
-        <v>398</v>
       </c>
       <c r="L9" s="25">
         <v>201503</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N9" s="25">
         <v>2</v>
       </c>
       <c r="O9" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="P9" s="25" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>446</v>
+      </c>
+      <c r="R9" s="25" t="s">
+        <v>447</v>
+      </c>
+      <c r="S9" s="25" t="s">
+        <v>448</v>
+      </c>
+      <c r="T9" s="25" t="s">
         <v>401</v>
       </c>
-      <c r="P9" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="Q9" s="25" t="s">
-        <v>447</v>
-      </c>
-      <c r="R9" s="25" t="s">
-        <v>448</v>
-      </c>
-      <c r="S9" s="25" t="s">
+      <c r="U9" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="V9" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="W9" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="X9" s="25" t="s">
         <v>449</v>
       </c>
-      <c r="T9" s="25" t="s">
-        <v>402</v>
-      </c>
-      <c r="U9" s="25" t="s">
-        <v>403</v>
-      </c>
-      <c r="V9" s="25" t="s">
-        <v>404</v>
-      </c>
-      <c r="W9" s="25" t="s">
+      <c r="Y9" s="25" t="s">
         <v>405</v>
       </c>
-      <c r="X9" s="25" t="s">
+      <c r="Z9" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="AA9" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="AB9" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="AC9" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="AD9" s="25" t="s">
         <v>450</v>
       </c>
-      <c r="Y9" s="25" t="s">
-        <v>406</v>
-      </c>
-      <c r="Z9" s="25" t="s">
-        <v>407</v>
-      </c>
-      <c r="AA9" s="25" t="s">
-        <v>408</v>
-      </c>
-      <c r="AB9" s="25" t="s">
+      <c r="AE9" s="25" t="s">
         <v>409</v>
       </c>
-      <c r="AC9" s="25" t="s">
-        <v>408</v>
-      </c>
-      <c r="AD9" s="25" t="s">
+      <c r="AF9" s="25" t="s">
         <v>451</v>
       </c>
-      <c r="AE9" s="25" t="s">
+      <c r="AG9" s="25" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH9" s="25" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI9" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK9" s="25" t="s">
+        <v>456</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>457</v>
+      </c>
+      <c r="AM9" s="25" t="s">
+        <v>458</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>459</v>
+      </c>
+      <c r="AO9" t="s">
         <v>410</v>
-      </c>
-      <c r="AF9" s="25" t="s">
-        <v>452</v>
-      </c>
-      <c r="AG9" s="25" t="s">
-        <v>453</v>
-      </c>
-      <c r="AH9" s="25" t="s">
-        <v>454</v>
-      </c>
-      <c r="AI9" s="25" t="s">
-        <v>455</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>456</v>
-      </c>
-      <c r="AK9" s="25" t="s">
-        <v>457</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>458</v>
-      </c>
-      <c r="AM9" s="25" t="s">
-        <v>459</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>460</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>411</v>
       </c>
       <c r="AP9">
         <v>30</v>
       </c>
       <c r="AQ9" t="s">
+        <v>460</v>
+      </c>
+      <c r="AR9" t="s">
         <v>461</v>
       </c>
-      <c r="AR9" t="s">
-        <v>462</v>
-      </c>
       <c r="AS9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -5456,20 +5477,20 @@
     </row>
     <row r="11" spans="1:45">
       <c r="B11" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C11" s="72" t="s">
         <v>394</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="D11" s="25" t="s">
         <v>395</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>396</v>
-      </c>
       <c r="E11" s="25" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J11" s="73"/>
       <c r="K11" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L11" s="25">
         <v>201504</v>
@@ -5478,16 +5499,16 @@
         <v>3</v>
       </c>
       <c r="T11" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="U11" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y11" s="25" t="s">
         <v>422</v>
       </c>
-      <c r="U11" s="25" t="s">
-        <v>403</v>
-      </c>
-      <c r="Y11" s="25" t="s">
+      <c r="AS11" t="s">
         <v>423</v>
-      </c>
-      <c r="AS11" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -5499,26 +5520,26 @@
         <v>3</v>
       </c>
       <c r="B13" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C13" s="72" t="s">
         <v>394</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="D13" s="25" t="s">
         <v>395</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>396</v>
-      </c>
       <c r="E13" s="25" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J13" s="73"/>
       <c r="K13" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="M13" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -5526,70 +5547,70 @@
         <v>4</v>
       </c>
       <c r="B14" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C14" s="72" t="s">
         <v>394</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="D14" s="25" t="s">
         <v>395</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="E14" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>396</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>426</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="G14" s="25" t="s">
+      <c r="I14" s="72" t="s">
+        <v>399</v>
+      </c>
+      <c r="J14" s="73" t="s">
+        <v>427</v>
+      </c>
+      <c r="K14" s="25" t="s">
         <v>397</v>
-      </c>
-      <c r="I14" s="72" t="s">
-        <v>400</v>
-      </c>
-      <c r="J14" s="73" t="s">
-        <v>428</v>
-      </c>
-      <c r="K14" s="25" t="s">
-        <v>398</v>
       </c>
       <c r="L14" s="25">
         <v>201504</v>
       </c>
       <c r="M14" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N14" s="25">
         <v>1</v>
       </c>
       <c r="O14" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="T14" s="25" t="s">
         <v>401</v>
       </c>
-      <c r="T14" s="25" t="s">
+      <c r="U14" s="25" t="s">
         <v>402</v>
       </c>
-      <c r="U14" s="25" t="s">
+      <c r="V14" s="25" t="s">
         <v>403</v>
       </c>
-      <c r="V14" s="25" t="s">
-        <v>404</v>
-      </c>
       <c r="W14" s="25" t="s">
+        <v>428</v>
+      </c>
+      <c r="Y14" s="25" t="s">
         <v>429</v>
       </c>
-      <c r="Y14" s="25" t="s">
+      <c r="AD14" s="25" t="s">
         <v>430</v>
       </c>
-      <c r="AD14" s="25" t="s">
-        <v>431</v>
-      </c>
       <c r="AO14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AP14">
         <v>20</v>
       </c>
       <c r="AS14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -5630,7 +5651,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="44" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -5640,7 +5661,7 @@
     </row>
     <row r="2" spans="1:6" ht="15">
       <c r="A2" s="47" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -5661,39 +5682,39 @@
         <v>170</v>
       </c>
       <c r="B4" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="70">
       <c r="A5" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5706,7 +5727,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -5719,19 +5740,19 @@
         <v>172</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D8" s="57" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E8" s="57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F8" s="63" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5739,13 +5760,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>413</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="E9" s="25" t="s">
         <v>414</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5753,10 +5774,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E10" s="25">
         <v>60</v>
@@ -5764,7 +5785,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -5796,7 +5817,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18">
       <c r="A1" s="44" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -5820,7 +5841,7 @@
     </row>
     <row r="2" spans="1:20" s="18" customFormat="1" ht="15">
       <c r="A2" s="47" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -5869,152 +5890,152 @@
         <v>170</v>
       </c>
       <c r="B4" s="64" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G4" s="64" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H4" s="64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I4" s="64" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J4" s="64" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K4" s="64" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L4" s="64" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M4" s="66" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="N4" s="66" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="O4" s="64" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="P4" s="64" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q4" s="64" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="R4" s="64" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="S4" s="64" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="T4" s="69" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="18" customFormat="1" ht="224">
       <c r="A5" s="50" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G5" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I5" s="41" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J5" s="41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K5" s="41" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M5" s="42" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N5" s="34" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O5" s="34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Q5" s="34" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="R5" s="34" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S5" s="34" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="T5" s="51" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="18" customFormat="1" ht="28">
       <c r="A6" s="52"/>
       <c r="B6" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C6" s="35"/>
       <c r="D6" s="35" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F6" s="35"/>
       <c r="G6" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
       <c r="M6" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N6" s="35"/>
       <c r="O6" s="36"/>
@@ -6022,13 +6043,13 @@
       <c r="Q6" s="36"/>
       <c r="R6" s="36"/>
       <c r="S6" s="36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="T6" s="70"/>
     </row>
     <row r="7" spans="1:20" s="18" customFormat="1">
       <c r="A7" s="54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -6048,7 +6069,7 @@
       <c r="Q7" s="37"/>
       <c r="R7" s="37"/>
       <c r="S7" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T7" s="55"/>
     </row>
@@ -6057,61 +6078,61 @@
         <v>172</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D8" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="E8" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="F8" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="G8" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="G8" s="57" t="s">
-        <v>350</v>
-      </c>
       <c r="H8" s="57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K8" s="57" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M8" s="57" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N8" s="57" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="P8" s="57" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Q8" s="57" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R8" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S8" s="58" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="T8" s="59" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -6122,19 +6143,19 @@
         <v>2</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>416</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="E9" s="25" t="s">
         <v>417</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="G9" s="25" t="s">
         <v>418</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>419</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>420</v>
       </c>
       <c r="I9" s="25">
         <v>2</v>
@@ -6143,7 +6164,7 @@
         <v>2015</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="S9" s="25">
         <v>100</v>
@@ -6157,13 +6178,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>434</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="E10" s="25" t="s">
         <v>435</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -6174,19 +6195,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="25" t="s">
+        <v>436</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>437</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="E12" s="25" t="s">
         <v>438</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="G12" s="25" t="s">
         <v>439</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="H12" s="25" t="s">
         <v>440</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>441</v>
       </c>
       <c r="I12" s="25">
         <v>3</v>
@@ -6195,13 +6216,13 @@
         <v>2015</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="S12" s="25">
         <v>410</v>
       </c>
       <c r="T12" s="25" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>